<commit_message>
Aggiornato file Ore al 15/12/2017
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23746b98e795164b/Documenti/Universitas/INFORMATICA/II Anno/Programmazione ad oggetti/2017/oop_project/MasterBranch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="EA8489ADAD643665BE42CD4F9B4AF3136FA26FAB" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{129FCFCE-CCC9-4E1C-A580-AE1745C1F6DC}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="EA8489ADAD643665BE42CD4F9B4AF3136FA26FAB" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{16D65F72-9648-4079-8641-344D304CB6D6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="18514" windowHeight="8057" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="18514" windowHeight="8057" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>rielaborazione gerarchia, tentativi di combinazione</t>
+  </si>
+  <si>
+    <t>Definizione comportamento combinazione, probabilita</t>
   </si>
 </sst>
 </file>
@@ -96,7 +99,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,14 +114,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -158,7 +153,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -473,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -484,6 +480,7 @@
     <col min="1" max="1" width="23.61328125" style="9" customWidth="1"/>
     <col min="3" max="3" width="23.61328125" style="4" customWidth="1"/>
     <col min="4" max="4" width="9.23046875" style="5"/>
+    <col min="9" max="9" width="21.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
@@ -521,19 +518,19 @@
         <v>8</v>
       </c>
       <c r="D2" s="5">
-        <v>2.0833333333333299</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F2" s="5">
         <f>SUMIFS(D:D,B:B,"Giovanni")</f>
-        <v>5.4166666666666634</v>
+        <v>0.58333333333333326</v>
       </c>
       <c r="G2" s="5">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
-        <v>4.3472222222222232</v>
-      </c>
-      <c r="I2" s="5">
-        <f>SUM(F2+G2)</f>
-        <v>9.7638888888888857</v>
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="I2" s="11">
+        <f>F2+G2</f>
+        <v>1.0972222222222223</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
@@ -547,7 +544,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="5">
-        <v>2.0833333333333299</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.4">
@@ -561,7 +558,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="5">
-        <v>2.1041666666666701</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="53.6" customHeight="1" x14ac:dyDescent="0.4">
@@ -575,7 +572,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="5">
-        <v>3.125</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="42.9" customHeight="1" x14ac:dyDescent="0.4">
@@ -688,6 +685,34 @@
       </c>
       <c r="D13" s="5">
         <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A14" s="9">
+        <v>43084</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A15" s="9">
+        <v>43084</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.16666666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ho continuato a scrivere codice. Classe oggetto con tutte le stats inserite e ho implementato tutti i metodi di servizio. Ho iniziato a scrivere qualcosa riguardo combina, ma con poco successo. Ho inserito un file 'operazioniMath' dove magari potremo mettere dentro tutte le funzioni matematiche che useremo... Ma vedremo che fare.
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="EA8489ADAD643665BE42CD4F9B4AF3136FA26FAB" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{16D65F72-9648-4079-8641-344D304CB6D6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="18514" windowHeight="8057" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="18514" windowHeight="8057" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -88,6 +87,9 @@
   </si>
   <si>
     <t>Definizione comportamento combinazione, probabilita</t>
+  </si>
+  <si>
+    <t>Continuato a scrivere codice. Classe oggetto riempita con tutti I parametri e le funzioni di servizio</t>
   </si>
 </sst>
 </file>
@@ -469,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -522,7 +524,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUMIFS(D:D,B:B,"Giovanni")</f>
-        <v>0.58333333333333326</v>
+        <v>0.62499999999999989</v>
       </c>
       <c r="G2" s="5">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
@@ -530,7 +532,7 @@
       </c>
       <c r="I2" s="11">
         <f>F2+G2</f>
-        <v>1.0972222222222223</v>
+        <v>1.1388888888888888</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
@@ -713,6 +715,20 @@
       </c>
       <c r="D15" s="5">
         <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A16" s="9">
+        <v>43086</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="5">
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornato file Ore con orario del 18/12 e del 19/12. Manca ancora la rendicontazione del 19/12 per Mirko.
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,8 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="14" documentId="83C89C06F15F8D4B876FFCBA93B71475EF30F2CE" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{F408EA26-BAE2-4B4B-94E0-D6C6B5CE009C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="18514" windowHeight="8057" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="18514" windowHeight="8057" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -90,6 +91,12 @@
   </si>
   <si>
     <t>Continuato a scrivere codice. Classe oggetto riempita con tutti I parametri e le funzioni di servizio</t>
+  </si>
+  <si>
+    <t>Scrittura metodo combina, crea, ricicla</t>
+  </si>
+  <si>
+    <t>Debug di crea :(</t>
   </si>
 </sst>
 </file>
@@ -471,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -522,17 +529,17 @@
       <c r="D2" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="11">
         <f>SUMIFS(D:D,B:B,"Giovanni")</f>
-        <v>0.62499999999999989</v>
-      </c>
-      <c r="G2" s="5">
+        <v>0.87499999999999989</v>
+      </c>
+      <c r="G2" s="11">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
-        <v>0.51388888888888895</v>
+        <v>0.65972222222222232</v>
       </c>
       <c r="I2" s="11">
         <f>F2+G2</f>
-        <v>1.1388888888888888</v>
+        <v>1.5347222222222223</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
@@ -729,6 +736,48 @@
       </c>
       <c r="D16" s="5">
         <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A17" s="9">
+        <v>43087</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.14583333333333334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A18" s="9">
+        <v>43087</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.14583333333333334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" s="9">
+        <v>43088</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.10416666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornato file Ore al 20/12/2017 pomeriggio
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="83C89C06F15F8D4B876FFCBA93B71475EF30F2CE" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{F408EA26-BAE2-4B4B-94E0-D6C6B5CE009C}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="83C89C06F15F8D4B876FFCBA93B71475EF30F2CE" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{12943FAE-D5AA-491D-BD88-57C14D4F97C6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4200" windowWidth="18514" windowHeight="8057" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="18514" windowHeight="8057" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Debug di crea :(</t>
+  </si>
+  <si>
+    <t>Rinomina metodi</t>
+  </si>
+  <si>
+    <t>creazione namespace mathOp per operazioni su mappe e altro.</t>
   </si>
 </sst>
 </file>
@@ -478,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -531,15 +537,15 @@
       </c>
       <c r="F2" s="11">
         <f>SUMIFS(D:D,B:B,"Giovanni")</f>
-        <v>0.87499999999999989</v>
+        <v>0.95833333333333326</v>
       </c>
       <c r="G2" s="11">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
-        <v>0.65972222222222232</v>
+        <v>0.68055555555555569</v>
       </c>
       <c r="I2" s="11">
         <f>F2+G2</f>
-        <v>1.5347222222222223</v>
+        <v>1.6388888888888888</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
@@ -778,6 +784,34 @@
       </c>
       <c r="D19" s="5">
         <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" s="9">
+        <v>43088</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="5">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A21" s="9">
+        <v>43089</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="5">
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ore aggiornato al 08/01 al pomeriggio
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="83C89C06F15F8D4B876FFCBA93B71475EF30F2CE" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{12943FAE-D5AA-491D-BD88-57C14D4F97C6}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="83C89C06F15F8D4B876FFCBA93B71475EF30F2CE" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{35DCD08D-C44C-43B2-9F93-C03AB97DB5AF}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4800" windowWidth="18514" windowHeight="8057" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>creazione namespace mathOp per operazioni su mappe e altro.</t>
+  </si>
+  <si>
+    <t>discussione implementazioni e sistemato virtual in tutti I metodi. Aggiunte firme alle classi mancanti. Aggiunti branch personali.</t>
   </si>
 </sst>
 </file>
@@ -484,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -537,15 +540,15 @@
       </c>
       <c r="F2" s="11">
         <f>SUMIFS(D:D,B:B,"Giovanni")</f>
-        <v>0.95833333333333326</v>
+        <v>1.1041666666666665</v>
       </c>
       <c r="G2" s="11">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
-        <v>0.68055555555555569</v>
+        <v>0.82638888888888906</v>
       </c>
       <c r="I2" s="11">
         <f>F2+G2</f>
-        <v>1.6388888888888888</v>
+        <v>1.9305555555555556</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
@@ -812,6 +815,34 @@
       </c>
       <c r="D21" s="5">
         <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A22" s="9">
+        <v>42743</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0.14583333333333334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A23" s="9">
+        <v>42743</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.14583333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rendicontazione ore al 10/01/2018 sera
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="83C89C06F15F8D4B876FFCBA93B71475EF30F2CE" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{35DCD08D-C44C-43B2-9F93-C03AB97DB5AF}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="83C89C06F15F8D4B876FFCBA93B71475EF30F2CE" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{6DCD29DC-1477-4E42-A9E2-6ECCB13F3E70}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="18514" windowHeight="8057" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
+    <workbookView xWindow="0" yWindow="5400" windowWidth="18516" windowHeight="8052" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>discussione implementazioni e sistemato virtual in tutti I metodi. Aggiunte firme alle classi mancanti. Aggiunti branch personali.</t>
+  </si>
+  <si>
+    <t>Implementatata bozza grafica calcolatrice con 6 bottoni, testo e icone</t>
   </si>
 </sst>
 </file>
@@ -117,7 +120,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +135,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -173,6 +184,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -487,21 +499,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.61328125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="23.61328125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.23046875" style="5"/>
-    <col min="9" max="9" width="21.4609375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" style="5"/>
+    <col min="9" max="9" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -525,7 +537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>43075</v>
       </c>
@@ -544,14 +556,14 @@
       </c>
       <c r="G2" s="11">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
-        <v>0.82638888888888906</v>
-      </c>
-      <c r="I2" s="11">
+        <v>0.99305555555555569</v>
+      </c>
+      <c r="I2" s="12">
         <f>F2+G2</f>
-        <v>1.9305555555555556</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+        <v>2.0972222222222223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>43075</v>
       </c>
@@ -565,7 +577,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>43076</v>
       </c>
@@ -579,7 +591,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="53.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="53.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>43076</v>
       </c>
@@ -593,7 +605,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="42.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="42.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>43079</v>
       </c>
@@ -607,7 +619,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>43080</v>
       </c>
@@ -621,7 +633,7 @@
         <v>2.0833333333333301E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="39.450000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" ht="39.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>43080</v>
       </c>
@@ -635,7 +647,7 @@
         <v>4.1666666666666699E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>43081</v>
       </c>
@@ -649,7 +661,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>43081</v>
       </c>
@@ -663,7 +675,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>43081</v>
       </c>
@@ -677,7 +689,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>43082</v>
       </c>
@@ -691,7 +703,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>43084</v>
       </c>
@@ -705,7 +717,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>43084</v>
       </c>
@@ -719,7 +731,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>43084</v>
       </c>
@@ -733,7 +745,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>43086</v>
       </c>
@@ -747,7 +759,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>43087</v>
       </c>
@@ -761,7 +773,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>43087</v>
       </c>
@@ -775,7 +787,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>43088</v>
       </c>
@@ -789,7 +801,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>43088</v>
       </c>
@@ -803,7 +815,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>43089</v>
       </c>
@@ -817,7 +829,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>42743</v>
       </c>
@@ -831,7 +843,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>42743</v>
       </c>
@@ -843,6 +855,20 @@
       </c>
       <c r="D23" s="5">
         <v>0.14583333333333334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="9">
+        <v>42745</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.16666666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornato file  Ore al 16/01/2018 sera
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="83C89C06F15F8D4B876FFCBA93B71475EF30F2CE" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{6DCD29DC-1477-4E42-A9E2-6ECCB13F3E70}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="107_{2E16341A-3EBC-4546-BBBF-0B0E32DD5606}" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{8C95CA4F-0EBB-460D-9BF7-C40579D0A465}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="18516" windowHeight="8052" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
+    <workbookView xWindow="0" yWindow="6000" windowWidth="18514" windowHeight="8049" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Implementatata bozza grafica calcolatrice con 6 bottoni, testo e icone</t>
+  </si>
+  <si>
+    <t>Compreso ed implementato il pattern MVC. Iniziato a modellare il progetto secondo questo standard.</t>
   </si>
 </sst>
 </file>
@@ -120,7 +123,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,14 +138,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -184,7 +179,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="46" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -499,21 +494,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" style="5"/>
-    <col min="9" max="9" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.69140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="23.69140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.23046875" style="5"/>
+    <col min="9" max="9" width="21.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -537,7 +532,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="9">
         <v>43075</v>
       </c>
@@ -552,7 +547,7 @@
       </c>
       <c r="F2" s="11">
         <f>SUMIFS(D:D,B:B,"Giovanni")</f>
-        <v>1.1041666666666665</v>
+        <v>1.1874999999999998</v>
       </c>
       <c r="G2" s="11">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
@@ -560,10 +555,10 @@
       </c>
       <c r="I2" s="12">
         <f>F2+G2</f>
-        <v>2.0972222222222223</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2.1805555555555554</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="9">
         <v>43075</v>
       </c>
@@ -577,7 +572,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="9">
         <v>43076</v>
       </c>
@@ -591,7 +586,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="53.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="53.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="9">
         <v>43076</v>
       </c>
@@ -605,7 +600,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="42.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="42.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="9">
         <v>43079</v>
       </c>
@@ -619,7 +614,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" s="9">
         <v>43080</v>
       </c>
@@ -633,7 +628,7 @@
         <v>2.0833333333333301E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="39.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="39.450000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="9">
         <v>43080</v>
       </c>
@@ -647,7 +642,7 @@
         <v>4.1666666666666699E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A9" s="9">
         <v>43081</v>
       </c>
@@ -661,7 +656,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A10" s="9">
         <v>43081</v>
       </c>
@@ -675,7 +670,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="9">
         <v>43081</v>
       </c>
@@ -689,7 +684,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="9">
         <v>43082</v>
       </c>
@@ -703,7 +698,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="9">
         <v>43084</v>
       </c>
@@ -717,7 +712,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="9">
         <v>43084</v>
       </c>
@@ -731,7 +726,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A15" s="9">
         <v>43084</v>
       </c>
@@ -745,7 +740,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A16" s="9">
         <v>43086</v>
       </c>
@@ -759,7 +754,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" s="9">
         <v>43087</v>
       </c>
@@ -773,7 +768,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A18" s="9">
         <v>43087</v>
       </c>
@@ -787,7 +782,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" s="9">
         <v>43088</v>
       </c>
@@ -801,7 +796,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" s="9">
         <v>43088</v>
       </c>
@@ -815,7 +810,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A21" s="9">
         <v>43089</v>
       </c>
@@ -829,7 +824,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A22" s="9">
         <v>42743</v>
       </c>
@@ -843,9 +838,9 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A23" s="9">
-        <v>42743</v>
+        <v>43108</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
@@ -857,9 +852,9 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A24" s="9">
-        <v>42745</v>
+        <v>43110</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
@@ -869,6 +864,20 @@
       </c>
       <c r="D24" s="5">
         <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A25" s="9">
+        <v>43116</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="5">
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornato file Ore al 18/01/2018
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="107_{2E16341A-3EBC-4546-BBBF-0B0E32DD5606}" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{8C95CA4F-0EBB-460D-9BF7-C40579D0A465}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="4B4417EB997A706DE2515FD680B1F8F43A6FB060" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{FF4A493B-1B27-44EB-A4D4-4045C6000D4A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6000" windowWidth="18514" windowHeight="8049" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
+    <workbookView xWindow="0" yWindow="7200" windowWidth="18516" windowHeight="8052" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -112,6 +112,24 @@
   </si>
   <si>
     <t>Compreso ed implementato il pattern MVC. Iniziato a modellare il progetto secondo questo standard.</t>
+  </si>
+  <si>
+    <t>Ore di studio</t>
+  </si>
+  <si>
+    <t>Implementata selezione di oggetto con suo conseguente settaggio ed allocazione in memoria. Utili: distinzione per MVC; far apparire e sparire un widget; gestione della memoria in maniera condivisa: per la memoria temporanea si usa il controller, che viene flushato alla fine di ogni settaggio; memoria non volatile nel modello, a meno di clear. Nel modello rimane la storia dei calcoli, fino a quando si vuole -&gt; facile implementazione della memoria 'a lato'. Da implementare ora nel master</t>
+  </si>
+  <si>
+    <t>studio di Qt per gestione MVC</t>
+  </si>
+  <si>
+    <t>Lavoro</t>
+  </si>
+  <si>
+    <t>Studio</t>
+  </si>
+  <si>
+    <t>studio di Qt per gestione grafica</t>
   </si>
 </sst>
 </file>
@@ -123,7 +141,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +157,22 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -148,7 +182,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -156,11 +190,72 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -178,8 +273,16 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -494,21 +597,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.69140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="23.69140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.23046875" style="5"/>
-    <col min="9" max="9" width="21.4609375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" style="5"/>
+    <col min="5" max="5" width="11.6640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -521,18 +625,22 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="18"/>
+      <c r="J1" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>43075</v>
       </c>
@@ -545,20 +653,24 @@
       <c r="D2" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="13">
         <f>SUMIFS(D:D,B:B,"Giovanni")</f>
-        <v>1.1874999999999998</v>
-      </c>
-      <c r="G2" s="11">
+        <v>1.2291666666666665</v>
+      </c>
+      <c r="H2" s="13">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
         <v>0.99305555555555569</v>
       </c>
-      <c r="I2" s="12">
-        <f>F2+G2</f>
-        <v>2.1805555555555554</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I2" s="14"/>
+      <c r="J2" s="17">
+        <f>G2+H2</f>
+        <v>2.2222222222222223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>43075</v>
       </c>
@@ -571,8 +683,24 @@
       <c r="D3" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F3" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="13">
+        <f>SUMIFS(E:E,B:B,"Giovanni")</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H3" s="13">
+        <f>SUMIFS(E:E,B:B,"Mirko")</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I3" s="14"/>
+      <c r="J3" s="17">
+        <f>G3+H3</f>
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>43076</v>
       </c>
@@ -586,7 +714,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="53.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="53.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>43076</v>
       </c>
@@ -599,8 +727,9 @@
       <c r="D5" s="5">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="42.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" ht="42.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>43079</v>
       </c>
@@ -614,7 +743,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>43080</v>
       </c>
@@ -628,7 +757,7 @@
         <v>2.0833333333333301E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="39.450000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="39.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>43080</v>
       </c>
@@ -642,7 +771,7 @@
         <v>4.1666666666666699E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>43081</v>
       </c>
@@ -656,7 +785,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>43081</v>
       </c>
@@ -670,7 +799,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>43081</v>
       </c>
@@ -684,7 +813,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>43082</v>
       </c>
@@ -697,8 +826,9 @@
       <c r="D12" s="10">
         <v>1.3888888888888888E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>43084</v>
       </c>
@@ -712,7 +842,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>43084</v>
       </c>
@@ -726,7 +856,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>43084</v>
       </c>
@@ -740,7 +870,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>43086</v>
       </c>
@@ -754,7 +884,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>43087</v>
       </c>
@@ -768,7 +898,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>43087</v>
       </c>
@@ -782,7 +912,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>43088</v>
       </c>
@@ -796,7 +926,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>43088</v>
       </c>
@@ -810,7 +940,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>43089</v>
       </c>
@@ -824,7 +954,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>42743</v>
       </c>
@@ -838,7 +968,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>43108</v>
       </c>
@@ -852,7 +982,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>43110</v>
       </c>
@@ -866,7 +996,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <v>43116</v>
       </c>
@@ -878,6 +1008,48 @@
       </c>
       <c r="D25" s="5">
         <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A26" s="9">
+        <v>43118</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="5">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="9">
+        <v>43118</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="9">
+        <v>43118</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0.16666666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornato file ore al 21/01/2018 sera. Mancano le ore di mirko?
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\GiovanniBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="4B4417EB997A706DE2515FD680B1F8F43A6FB060" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{FF4A493B-1B27-44EB-A4D4-4045C6000D4A}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="4B4417EB997A706DE2515FD680B1F8F43A6FB060" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{0DEF427A-FFB6-459E-96D6-FF52E544AE8C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7200" windowWidth="18516" windowHeight="8052" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
+    <workbookView xWindow="0" yWindow="7800" windowWidth="18516" windowHeight="8052" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>studio di Qt per gestione grafica</t>
+  </si>
+  <si>
+    <t>Implementati tasti gestione memoria. Implementato uso di combina. Cambiata implementazione della memoria nel modello ed alcuni metodi del controller.</t>
   </si>
 </sst>
 </file>
@@ -597,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,7 +661,7 @@
       </c>
       <c r="G2" s="13">
         <f>SUMIFS(D:D,B:B,"Giovanni")</f>
-        <v>1.2291666666666665</v>
+        <v>1.4791666666666665</v>
       </c>
       <c r="H2" s="13">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
@@ -667,7 +670,7 @@
       <c r="I2" s="14"/>
       <c r="J2" s="17">
         <f>G2+H2</f>
-        <v>2.2222222222222223</v>
+        <v>2.4722222222222223</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -688,7 +691,7 @@
       </c>
       <c r="G3" s="13">
         <f>SUMIFS(E:E,B:B,"Giovanni")</f>
-        <v>0.41666666666666669</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="H3" s="13">
         <f>SUMIFS(E:E,B:B,"Mirko")</f>
@@ -697,7 +700,7 @@
       <c r="I3" s="14"/>
       <c r="J3" s="17">
         <f>G3+H3</f>
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -1050,6 +1053,23 @@
       </c>
       <c r="E28" s="5">
         <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="9">
+        <v>43121</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E29" s="5">
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sistemate operazioni binarie e logica calcolatrice
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\GiovanniBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="4B4417EB997A706DE2515FD680B1F8F43A6FB060" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{0DEF427A-FFB6-459E-96D6-FF52E544AE8C}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="4B4417EB997A706DE2515FD680B1F8F43A6FB060" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{A5E0E39D-CD4C-482E-827D-3EF0E6B82EC6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7800" windowWidth="18516" windowHeight="8052" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
+    <workbookView xWindow="0" yWindow="8400" windowWidth="18516" windowHeight="8052" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Implementati tasti gestione memoria. Implementato uso di combina. Cambiata implementazione della memoria nel modello ed alcuni metodi del controller.</t>
+  </si>
+  <si>
+    <t>progresso e test/studio</t>
+  </si>
+  <si>
+    <t>sistemato metodi clear back display</t>
   </si>
 </sst>
 </file>
@@ -600,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,12 +671,12 @@
       </c>
       <c r="H2" s="13">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
-        <v>0.99305555555555569</v>
+        <v>1.1388888888888891</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="17">
         <f>G2+H2</f>
-        <v>2.4722222222222223</v>
+        <v>2.6180555555555554</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -695,12 +701,12 @@
       </c>
       <c r="H3" s="13">
         <f>SUMIFS(E:E,B:B,"Mirko")</f>
-        <v>0.16666666666666666</v>
+        <v>0.4375</v>
       </c>
       <c r="I3" s="14"/>
       <c r="J3" s="17">
         <f>G3+H3</f>
-        <v>0.625</v>
+        <v>0.89583333333333337</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -1055,21 +1061,55 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
+        <v>43120</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="5">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="9">
         <v>43121</v>
       </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D30" s="5">
         <v>0.25</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E30" s="5">
         <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="9">
+        <v>43121</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="5">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E31" s="5">
+        <v>6.25E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornato file ore progetto al 22/01
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\GiovanniBranch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="4B4417EB997A706DE2515FD680B1F8F43A6FB060" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{A5E0E39D-CD4C-482E-827D-3EF0E6B82EC6}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="4B4417EB997A706DE2515FD680B1F8F43A6FB060" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{2B41706E-2E5F-4F35-88BB-F945A7EF480D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8400" windowWidth="18516" windowHeight="8052" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
+    <workbookView xWindow="0" yWindow="9000" windowWidth="18516" windowHeight="8052" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>sistemato metodi clear back display</t>
+  </si>
+  <si>
+    <t>sistemato display con clear back scroll</t>
+  </si>
+  <si>
+    <t>sistemata logica calcolatrice</t>
   </si>
 </sst>
 </file>
@@ -606,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,16 +673,16 @@
       </c>
       <c r="G2" s="13">
         <f>SUMIFS(D:D,B:B,"Giovanni")</f>
-        <v>1.4791666666666665</v>
+        <v>1.6041666666666665</v>
       </c>
       <c r="H2" s="13">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
-        <v>1.1388888888888891</v>
+        <v>1.2638888888888891</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="17">
         <f>G2+H2</f>
-        <v>2.6180555555555554</v>
+        <v>2.8680555555555554</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -722,6 +728,7 @@
       <c r="D4" s="5">
         <v>0.10416666666666667</v>
       </c>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:10" ht="53.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
@@ -1110,6 +1117,34 @@
       </c>
       <c r="E31" s="5">
         <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="9">
+        <v>43122</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="9">
+        <v>43122</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="5">
+        <v>0.125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornato file orario. C'era una incongruenza nel mio calcolo, ora risolta. 22/01/2018
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="4B4417EB997A706DE2515FD680B1F8F43A6FB060" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{2B41706E-2E5F-4F35-88BB-F945A7EF480D}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="4B4417EB997A706DE2515FD680B1F8F43A6FB060" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{9E3C9303-908F-4A3F-ADF8-BD212849C030}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="9000" windowWidth="18516" windowHeight="8052" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1096,7 +1096,7 @@
         <v>35</v>
       </c>
       <c r="D30" s="5">
-        <v>0.25</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="E30" s="5">
         <v>4.1666666666666664E-2</v>
@@ -1144,7 +1144,7 @@
         <v>39</v>
       </c>
       <c r="D33" s="5">
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sistemata (!!!!) logica della calcolatrice. Forse è la volta buona: ora funziona tutto, per la parte di operazioni binarie. Sono da sistemare le operazioni unarie e tasto answer
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="4B4417EB997A706DE2515FD680B1F8F43A6FB060" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{9E3C9303-908F-4A3F-ADF8-BD212849C030}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9000" windowWidth="18516" windowHeight="8052" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
+    <workbookView xWindow="0" yWindow="9000" windowWidth="18514" windowHeight="8049" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -145,6 +144,9 @@
   </si>
   <si>
     <t>sistemata logica calcolatrice</t>
+  </si>
+  <si>
+    <t>implementazione metodo potenza</t>
   </si>
 </sst>
 </file>
@@ -612,22 +614,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" style="5"/>
-    <col min="5" max="5" width="11.6640625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.69140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="23.69140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.23046875" style="5"/>
+    <col min="5" max="5" width="11.69140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="21.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -655,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="9">
         <v>43075</v>
       </c>
@@ -677,15 +679,15 @@
       </c>
       <c r="H2" s="13">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
-        <v>1.2638888888888891</v>
+        <v>1.3055555555555558</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="17">
         <f>G2+H2</f>
-        <v>2.8680555555555554</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>2.9097222222222223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="9">
         <v>43075</v>
       </c>
@@ -715,7 +717,7 @@
         <v>0.89583333333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="9">
         <v>43076</v>
       </c>
@@ -730,7 +732,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:10" ht="53.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="53.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="9">
         <v>43076</v>
       </c>
@@ -745,7 +747,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:10" ht="42.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="42.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="9">
         <v>43079</v>
       </c>
@@ -759,7 +761,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="9">
         <v>43080</v>
       </c>
@@ -773,7 +775,7 @@
         <v>2.0833333333333301E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="39.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="39.450000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="9">
         <v>43080</v>
       </c>
@@ -787,7 +789,7 @@
         <v>4.1666666666666699E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A9" s="9">
         <v>43081</v>
       </c>
@@ -801,7 +803,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A10" s="9">
         <v>43081</v>
       </c>
@@ -815,7 +817,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="9">
         <v>43081</v>
       </c>
@@ -829,7 +831,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="9">
         <v>43082</v>
       </c>
@@ -844,7 +846,7 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="9">
         <v>43084</v>
       </c>
@@ -858,7 +860,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="9">
         <v>43084</v>
       </c>
@@ -872,7 +874,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A15" s="9">
         <v>43084</v>
       </c>
@@ -886,7 +888,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A16" s="9">
         <v>43086</v>
       </c>
@@ -900,7 +902,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" s="9">
         <v>43087</v>
       </c>
@@ -914,7 +916,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A18" s="9">
         <v>43087</v>
       </c>
@@ -928,7 +930,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="9">
         <v>43088</v>
       </c>
@@ -942,7 +944,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="9">
         <v>43088</v>
       </c>
@@ -956,7 +958,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A21" s="9">
         <v>43089</v>
       </c>
@@ -970,7 +972,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A22" s="9">
         <v>42743</v>
       </c>
@@ -984,7 +986,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A23" s="9">
         <v>43108</v>
       </c>
@@ -998,7 +1000,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A24" s="9">
         <v>43110</v>
       </c>
@@ -1012,7 +1014,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A25" s="9">
         <v>43116</v>
       </c>
@@ -1026,7 +1028,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="306" x14ac:dyDescent="0.4">
       <c r="A26" s="9">
         <v>43118</v>
       </c>
@@ -1040,7 +1042,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A27" s="9">
         <v>43118</v>
       </c>
@@ -1054,7 +1056,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A28" s="9">
         <v>43118</v>
       </c>
@@ -1068,7 +1070,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" s="9">
         <v>43120</v>
       </c>
@@ -1085,7 +1087,7 @@
         <v>0.20833333333333334</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="102" x14ac:dyDescent="0.4">
       <c r="A30" s="9">
         <v>43121</v>
       </c>
@@ -1102,7 +1104,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A31" s="9">
         <v>43121</v>
       </c>
@@ -1119,7 +1121,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" s="9">
         <v>43122</v>
       </c>
@@ -1133,7 +1135,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33" s="9">
         <v>43122</v>
       </c>
@@ -1145,6 +1147,20 @@
       </c>
       <c r="D33" s="5">
         <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A34" s="9">
+        <v>43124</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="5">
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornato file Ore con la rendicontazione al 01 mattina
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,8 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="22" documentId="58034407F900E122BC498223926013154D689624" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{5813385C-BFE8-4228-BDC4-FCD5FF800CC9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9000" windowWidth="18514" windowHeight="8049" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
+    <workbookView xWindow="0" yWindow="9000" windowWidth="18516" windowHeight="8052" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -147,6 +148,21 @@
   </si>
   <si>
     <t>implementazione metodo potenza</t>
+  </si>
+  <si>
+    <t>implementazione pulsante ricicla, potenzia da finire</t>
+  </si>
+  <si>
+    <t>implementazione metodi gerarchia</t>
+  </si>
+  <si>
+    <t>fine implementazione potenzia</t>
+  </si>
+  <si>
+    <t>crea e trasforma</t>
+  </si>
+  <si>
+    <t>implementazione crea</t>
   </si>
 </sst>
 </file>
@@ -272,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -300,6 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -614,22 +631,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.69140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="23.69140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.23046875" style="5"/>
-    <col min="5" max="5" width="11.69140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="21.4609375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" style="5"/>
+    <col min="5" max="5" width="11.6640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -657,7 +674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>43075</v>
       </c>
@@ -675,19 +692,19 @@
       </c>
       <c r="G2" s="13">
         <f>SUMIFS(D:D,B:B,"Giovanni")</f>
-        <v>1.6041666666666665</v>
+        <v>1.8124999999999998</v>
       </c>
       <c r="H2" s="13">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
-        <v>1.3055555555555558</v>
+        <v>1.5138888888888891</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="17">
         <f>G2+H2</f>
-        <v>2.9097222222222223</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+        <v>3.3263888888888888</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>43075</v>
       </c>
@@ -717,7 +734,7 @@
         <v>0.89583333333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>43076</v>
       </c>
@@ -732,7 +749,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:10" ht="53.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="53.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>43076</v>
       </c>
@@ -747,7 +764,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:10" ht="42.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="42.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>43079</v>
       </c>
@@ -761,7 +778,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>43080</v>
       </c>
@@ -775,7 +792,7 @@
         <v>2.0833333333333301E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="39.450000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="39.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>43080</v>
       </c>
@@ -789,7 +806,7 @@
         <v>4.1666666666666699E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>43081</v>
       </c>
@@ -803,7 +820,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>43081</v>
       </c>
@@ -817,7 +834,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>43081</v>
       </c>
@@ -831,7 +848,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>43082</v>
       </c>
@@ -846,7 +863,7 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>43084</v>
       </c>
@@ -860,7 +877,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>43084</v>
       </c>
@@ -874,7 +891,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>43084</v>
       </c>
@@ -888,7 +905,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>43086</v>
       </c>
@@ -902,7 +919,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>43087</v>
       </c>
@@ -916,7 +933,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>43087</v>
       </c>
@@ -930,7 +947,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>43088</v>
       </c>
@@ -944,7 +961,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>43088</v>
       </c>
@@ -958,7 +975,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>43089</v>
       </c>
@@ -972,7 +989,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>42743</v>
       </c>
@@ -986,7 +1003,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>43108</v>
       </c>
@@ -1000,7 +1017,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>43110</v>
       </c>
@@ -1014,7 +1031,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <v>43116</v>
       </c>
@@ -1028,7 +1045,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="306" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <v>43118</v>
       </c>
@@ -1042,7 +1059,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>43118</v>
       </c>
@@ -1056,7 +1073,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <v>43118</v>
       </c>
@@ -1070,7 +1087,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
         <v>43120</v>
       </c>
@@ -1087,7 +1104,7 @@
         <v>0.20833333333333334</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="102" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <v>43121</v>
       </c>
@@ -1104,7 +1121,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="9">
         <v>43121</v>
       </c>
@@ -1121,7 +1138,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
         <v>43122</v>
       </c>
@@ -1135,7 +1152,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
         <v>43122</v>
       </c>
@@ -1149,7 +1166,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="9">
         <v>43124</v>
       </c>
@@ -1162,6 +1179,79 @@
       <c r="D34" s="5">
         <v>4.1666666666666664E-2</v>
       </c>
+    </row>
+    <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="9">
+        <v>43130</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="5">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="9">
+        <v>43131</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="9">
+        <v>43131</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="5">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="9">
+        <v>43131</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="5">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="9">
+        <v>43132</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="5">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Aggiornato file ore al 01/01/2018. Mirko fai impressione
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,7 +8,6 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="58034407F900E122BC498223926013154D689624" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{5813385C-BFE8-4228-BDC4-FCD5FF800CC9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="9000" windowWidth="18516" windowHeight="8052" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -163,6 +162,9 @@
   </si>
   <si>
     <t>implementazione crea</t>
+  </si>
+  <si>
+    <t>gestione gerarchia</t>
   </si>
 </sst>
 </file>
@@ -316,7 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -692,16 +694,16 @@
       </c>
       <c r="G2" s="13">
         <f>SUMIFS(D:D,B:B,"Giovanni")</f>
-        <v>1.8124999999999998</v>
+        <v>2.1041666666666665</v>
       </c>
       <c r="H2" s="13">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
-        <v>1.5138888888888891</v>
+        <v>1.9513888888888891</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="17">
         <f>G2+H2</f>
-        <v>3.3263888888888888</v>
+        <v>4.0555555555555554</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1247,11 +1249,22 @@
         <v>45</v>
       </c>
       <c r="D39" s="5">
-        <v>4.1666666666666664E-2</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="21"/>
+      <c r="A40" s="21">
+        <v>43132</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="5">
+        <v>0.4375</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Aggiornato file orario con le ultime ore di lavoro del 01/02 di Gio
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -161,10 +161,10 @@
     <t>crea e trasforma</t>
   </si>
   <si>
-    <t>implementazione crea</t>
-  </si>
-  <si>
     <t>gestione gerarchia</t>
+  </si>
+  <si>
+    <t>implementazione crea, ripara, trasforma, distribuisci, duplica</t>
   </si>
 </sst>
 </file>
@@ -636,7 +636,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,7 +694,7 @@
       </c>
       <c r="G2" s="13">
         <f>SUMIFS(D:D,B:B,"Giovanni")</f>
-        <v>2.1041666666666665</v>
+        <v>2.1874999999999996</v>
       </c>
       <c r="H2" s="13">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
@@ -703,7 +703,7 @@
       <c r="I2" s="14"/>
       <c r="J2" s="17">
         <f>G2+H2</f>
-        <v>4.0555555555555554</v>
+        <v>4.1388888888888884</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1238,7 +1238,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="9">
         <v>43132</v>
       </c>
@@ -1246,10 +1246,10 @@
         <v>7</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D39" s="5">
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1260,7 +1260,7 @@
         <v>9</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D40" s="5">
         <v>0.4375</v>

</xml_diff>

<commit_message>
Ritocchi alla gerarchia, iniziata implementazione in java
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>implementazione crea, ripara, trasforma, distribuisci, duplica</t>
+  </si>
+  <si>
+    <t>ultimi ritocchi alla gerarchia, passaggio ai cpp</t>
+  </si>
+  <si>
+    <t>ultimi ritocchi alla gerarchia, passaggio ai cpp, prima implementazione di java</t>
   </si>
 </sst>
 </file>
@@ -633,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,16 +700,16 @@
       </c>
       <c r="G2" s="13">
         <f>SUMIFS(D:D,B:B,"Giovanni")</f>
-        <v>2.1874999999999996</v>
+        <v>2.6041666666666661</v>
       </c>
       <c r="H2" s="13">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
-        <v>1.9513888888888891</v>
+        <v>2.2847222222222223</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="17">
         <f>G2+H2</f>
-        <v>4.1388888888888884</v>
+        <v>4.8888888888888884</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1264,6 +1270,34 @@
       </c>
       <c r="D40" s="5">
         <v>0.4375</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="9">
+        <v>43133</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="9">
+        <v>43133</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="5">
+        <v>0.41666666666666669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornato Ore al 03/02/2018
</commit_message>
<xml_diff>
--- a/Ore.xlsx
+++ b/Ore.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9" documentId="35AE4C023FB1A2B27006FE50D2EA018E679F9B1E" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{481F313E-0823-46E7-94C6-39579734C4A3}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="9000" windowWidth="18516" windowHeight="8052" xr2:uid="{3CD30D49-6BFD-4BEA-9091-D17EA14F4E82}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -171,6 +172,12 @@
   </si>
   <si>
     <t>ultimi ritocchi alla gerarchia, passaggio ai cpp, prima implementazione di java</t>
+  </si>
+  <si>
+    <t>java e casi d'uso</t>
+  </si>
+  <si>
+    <t>fine implementazione java, risolti (molti) bug, inizio scrittura relazione e creazione immagini.</t>
   </si>
 </sst>
 </file>
@@ -639,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282688AE-2CDC-4833-B440-BF69D70CD3A2}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,16 +707,16 @@
       </c>
       <c r="G2" s="13">
         <f>SUMIFS(D:D,B:B,"Giovanni")</f>
-        <v>2.6041666666666661</v>
+        <v>3.0208333333333326</v>
       </c>
       <c r="H2" s="13">
         <f>SUMIFS(D:D,B:B,"Mirko")</f>
-        <v>2.2847222222222223</v>
+        <v>2.6388888888888888</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="17">
         <f>G2+H2</f>
-        <v>4.8888888888888884</v>
+        <v>5.6597222222222214</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1297,6 +1304,34 @@
         <v>48</v>
       </c>
       <c r="D42" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="9">
+        <v>43134</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="5">
+        <v>0.35416666666666669</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="9">
+        <v>43134</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="5">
         <v>0.41666666666666669</v>
       </c>
     </row>

</xml_diff>